<commit_message>
Handling the snesor working and testing simply communication via MQTT
</commit_message>
<xml_diff>
--- a/Hardware/Documentation/SensorList.xlsx
+++ b/Hardware/Documentation/SensorList.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Lp.</t>
   </si>
@@ -115,7 +115,10 @@
     <t>https://learn.adafruit.com/adafruit-bmp280-barometric-pressure-plus-temperature-sensor-breakout/overview</t>
   </si>
   <si>
-    <t xml:space="preserve">SPI Barometric Pressure &amp; Altitude </t>
+    <t>Pressure &amp; Altitude  &amp; Temperature</t>
+  </si>
+  <si>
+    <t>Altitude, Temperature not sending.</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,9 +510,10 @@
     <col min="4" max="4" width="62.140625" customWidth="1"/>
     <col min="5" max="5" width="89.85546875" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -528,8 +532,11 @@
       <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -544,8 +551,9 @@
         <v>18</v>
       </c>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -564,8 +572,11 @@
       <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -580,8 +591,9 @@
         <v>14</v>
       </c>
       <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -596,8 +608,9 @@
         <v>19</v>
       </c>
       <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -612,8 +625,9 @@
         <v>17</v>
       </c>
       <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -628,6 +642,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>